<commit_message>
Add a verification on eventHandler function for auto integer float numbers in qty inputs (cart.js file)
</commit_message>
<xml_diff>
--- a/plan_de_tests.xlsx
+++ b/plan_de_tests.xlsx
@@ -83,7 +83,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>displayProduct</t>
@@ -117,7 +117,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>saveProduct</t>
@@ -151,7 +151,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>displayConfirmationPopUp displayErrorPopUp</t>
@@ -194,7 +194,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>closePopUp</t>
@@ -228,7 +228,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>onClickAddToCart</t>
@@ -265,7 +265,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>refreshCart</t>
@@ -299,7 +299,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>displayCart</t>
@@ -333,7 +333,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>changeHandlerQty</t>
@@ -367,7 +367,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>calculateCartAmount</t>
@@ -401,7 +401,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>addEventListenerOnQtyInput</t>
@@ -435,7 +435,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>addEventListenerOnDeleteBtn</t>
@@ -469,7 +469,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>modifyCartQty</t>
@@ -500,7 +500,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>displayPopUpProductDeleted</t>
@@ -534,7 +534,7 @@
     <r>
       <rPr>
         <sz val="13"/>
-        <color indexed="11"/>
+        <color indexed="14"/>
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>deleteItem</t>
@@ -559,16 +559,16 @@
     <t>OK, Le produit est bien supprimé du local storage et de la page.</t>
   </si>
   <si>
-    <t>299 - 301</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color indexed="11"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>closeHelperSubmit</t>
+    <t>254 - 281</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="14"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>sendOrder</t>
     </r>
     <r>
       <rPr>
@@ -581,28 +581,29 @@
     </r>
   </si>
   <si>
-    <t>Permet de fermer le message d’erreur en cas de mauvaise quantité saisie.</t>
-  </si>
-  <si>
-    <t>Dans la page « panier », mettre une quantité erronée dans n’importe quel input Qté. Cliquer sur le bouton « commander !», un message d’erreur apparait puis disparait au bout de 1,8s.</t>
-  </si>
-  <si>
-    <t>Lors d’une mauvaise saisie de quantité, au clic sur le bouton « commander ! » un message apparait demandant de vérifier les quantités saisies. Elle se referme au bout de 1,8s.</t>
-  </si>
-  <si>
-    <t>OK, le message se ferme bien au bout de 1,8s.</t>
-  </si>
-  <si>
-    <t>254 - 281</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="13"/>
-        <color indexed="11"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>sendOrder</t>
+    <t>Lors du clic sur le bouton « Commander ! », le remplissage du formulaire de contact est analysé et validé selon les conditions des regExp mises en place. Une vérification des quantité est également effectuée. Si tout est bien rempli, alors un objet comprenant les informations de contact et les produits sont envoyés vers l’API. En réponse, un numéro de commande est réceptionné et stocké dans l’url de la page confirmation.</t>
+  </si>
+  <si>
+    <t>Appuyer sur le bouton « Commander ! ».</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les inputs des utilisateurs doivent être analysés et validés pour vérifier le format et le type de données avant l’envoi à l’API. Un message d’erreur apparait en cas de mauvais remplissage. Un numéro de commande est reçu via l’API, puis stockée dans l’url de la page confirmation vers laquelle l’utilisateur est redirigé.
+</t>
+  </si>
+  <si>
+    <t>OK, un message s’affiche bien en cas d’erreur de remplissage et l’envoi du formulaire est bloqué. En cas de réussite, le numéro de commande est stocké dans l’url de la page confirmation et l’utilisateur est redirigé vers celle-ci.</t>
+  </si>
+  <si>
+    <t>299 - 301</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color indexed="14"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>closeHelperSubmit</t>
     </r>
     <r>
       <rPr>
@@ -615,17 +616,16 @@
     </r>
   </si>
   <si>
-    <t>Lors du clic sur le bouton « Commander ! », le remplissage du formulaire de contact est analysé et validé selon les conditions des regExp mises en place. Une vérification des quantité est également effectuée. Si tout est bien rempli, alors un objet comprenant les informations de contact et les produits sont envoyés vers l’API. En réponse, un numéro de commande est réceptionné et stocké dans l’url de la page confirmation.</t>
-  </si>
-  <si>
-    <t>Appuyer sur le bouton « Commander ! ».</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les inputs des utilisateurs doivent être analysés et validés pour vérifier le format et le type de données avant l’envoi à l’API. Un message d’erreur apparait en cas de mauvais remplissage. Un numéro de commande est reçu via l’API, puis stockée dans l’url de la page confirmation vers laquelle l’utilisateur est redirigé.
-</t>
-  </si>
-  <si>
-    <t>OK, un message s’affiche bien en cas d’erreur de remplissage et l’envoi du formulaire est bloqué. En cas de réussite, le numéro de commande est stocké dans l’url de la page confirmation et l’utilisateur est redirigé vers celle-ci.</t>
+    <t>Permet de fermer le message d’erreur en cas de mauvaise quantité saisie.</t>
+  </si>
+  <si>
+    <t>Dans la page « panier », mettre une quantité erronée dans n’importe quel input Qté. Cliquer sur le bouton « commander !», un message d’erreur apparait puis disparait au bout de 1,8s.</t>
+  </si>
+  <si>
+    <t>Lors d’une mauvaise saisie de quantité, au clic sur le bouton « commander ! » un message apparait demandant de vérifier les quantités saisies. Elle se referme au bout de 1,8s.</t>
+  </si>
+  <si>
+    <t>OK, le message se ferme bien au bout de 1,8s.</t>
   </si>
   <si>
     <t>confirmation.js</t>
@@ -656,7 +656,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -700,6 +700,11 @@
     </font>
     <font>
       <sz val="13"/>
+      <color indexed="14"/>
+      <name val="Menlo Regular"/>
+    </font>
+    <font>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
@@ -731,12 +736,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
@@ -744,6 +743,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="16"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -1081,7 +1086,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1157,9 +1162,10 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffd9d9d9"/>
       <rgbColor rgb="ff99d3a9"/>
-      <rgbColor rgb="ff61afef"/>
+      <rgbColor rgb="ffa0c2f9"/>
       <rgbColor rgb="ffabb2bf"/>
       <rgbColor rgb="fffddd81"/>
+      <rgbColor rgb="ff61afef"/>
       <rgbColor rgb="ffffb680"/>
       <rgbColor rgb="fff4a19a"/>
       <rgbColor rgb="ffffffff"/>
@@ -1361,12 +1367,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1399,10 +1405,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1650,12 +1656,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1970,10 +1976,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Arial"/>
-            <a:ea typeface="Arial"/>
-            <a:cs typeface="Arial"/>
-            <a:sym typeface="Arial"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2233,12 +2239,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.60156" style="1" customWidth="1"/>
-    <col min="2" max="3" width="31.3047" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.3359" style="1" customWidth="1"/>
-    <col min="5" max="6" width="68.4922" style="1" customWidth="1"/>
-    <col min="7" max="7" width="67.7109" style="1" customWidth="1"/>
-    <col min="8" max="8" width="61.6797" style="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08594" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6016" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.6328" style="1" customWidth="1"/>
+    <col min="5" max="6" width="68.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="67.6719" style="1" customWidth="1"/>
+    <col min="8" max="8" width="61.6719" style="1" customWidth="1"/>
     <col min="9" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2654,12 +2661,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" ht="48.4" customHeight="1">
+    <row r="17" ht="114.5" customHeight="1">
       <c r="A17" s="18">
         <v>16</v>
       </c>
       <c r="B17" t="s" s="19">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="C17" t="s" s="20">
         <v>99</v>
@@ -2673,19 +2680,19 @@
       <c r="F17" t="s" s="22">
         <v>102</v>
       </c>
-      <c r="G17" t="s" s="22">
+      <c r="G17" t="s" s="26">
         <v>103</v>
       </c>
       <c r="H17" t="s" s="23">
         <v>104</v>
       </c>
     </row>
-    <row r="18" ht="114.5" customHeight="1">
+    <row r="18" ht="48.4" customHeight="1">
       <c r="A18" s="18">
         <v>17</v>
       </c>
       <c r="B18" t="s" s="19">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s" s="20">
         <v>105</v>
@@ -2699,7 +2706,7 @@
       <c r="F18" t="s" s="22">
         <v>108</v>
       </c>
-      <c r="G18" t="s" s="26">
+      <c r="G18" t="s" s="22">
         <v>109</v>
       </c>
       <c r="H18" t="s" s="23">

</xml_diff>